<commit_message>
Update Excel filename in bot.py from 'employees_data.xlsx' to 'employees.xlsx'
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evgeniizotov\Desktop\Файлы для бота\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Мэкс\Desktop\tg_ai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B003CB70-442B-4F94-B33D-B171EFF5FB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ADDB7C-AEA2-4B7E-B3D6-EC3C84ED6AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Tg_ID</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Марина</t>
+  </si>
+  <si>
+    <t>@IT_Svaha</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -164,12 +167,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,15 +474,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -549,7 +556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101700261</v>
       </c>
@@ -584,7 +591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -619,18 +626,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>836318110</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2">
-        <v>41385</v>
+        <v>45768</v>
       </c>
       <c r="E5">
         <v>856</v>
@@ -642,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="4">
-        <v>0.57708333333333295</v>
+        <v>0.88194444444444442</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>21</v>

</xml_diff>